<commit_message>
some adjustments based on risa's last comments
- figures adjsuted for consistency
- removed bad %N data and reran stats and created new tables
</commit_message>
<xml_diff>
--- a/analyses/tables/foliar_cn.xlsx
+++ b/analyses/tables/foliar_cn.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/mdi_pitchpine/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9774AE16-2356-864D-B004-B3E99D1C3BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC28ECA-FD05-5545-85FC-A152CFC5F664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="3360" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="8640" yWindow="7420" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foliar_cn" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -916,11 +916,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,11 +987,11 @@
       <c r="D3" s="2">
         <v>0.90837928277373003</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.118677517119908</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.73149160568215199</v>
+      <c r="E3" s="1">
+        <v>0.889412488061744</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.349024916001268</v>
       </c>
       <c r="G3" s="2">
         <v>1.3821282986871299</v>
@@ -1013,11 +1013,11 @@
       <c r="D4" s="2">
         <v>0.114775011255773</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.109426361660122</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.74177241855310905</v>
+      <c r="E4" s="1">
+        <v>4.2345550660915201</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.3502921115634703E-2</v>
       </c>
       <c r="G4" s="2">
         <v>0.635427849753332</v>
@@ -1039,11 +1039,11 @@
       <c r="D5" s="2">
         <v>0.83385500214015695</v>
       </c>
-      <c r="E5" s="2">
-        <v>2.83721015023915E-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.86671590359700301</v>
+      <c r="E5" s="1">
+        <v>0.59368054372753898</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.44370792261043501</v>
       </c>
       <c r="G5" s="2">
         <v>0.133852707542194</v>

</xml_diff>